<commit_message>
Inserindo link para bandeira
</commit_message>
<xml_diff>
--- a/datasets/info_futebol.xlsx
+++ b/datasets/info_futebol.xlsx
@@ -20,15 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t xml:space="preserve">Time</t>
   </si>
   <si>
-    <t xml:space="preserve">Pontuação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grupo paulistão</t>
+    <t xml:space="preserve">Pontuacao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grupo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imagem</t>
   </si>
   <si>
     <t xml:space="preserve">Santos</t>
@@ -37,58 +40,106 @@
     <t xml:space="preserve">A</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/santos.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Botafogo-SP</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/botasp.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inter de Limeira</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/intl.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bragantino</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/bragantino.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">São Paulo</t>
   </si>
   <si>
     <t xml:space="preserve">B</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/saopaulo.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Água Santa</t>
   </si>
   <si>
+    <t xml:space="preserve">https://static.wixstatic.com/media/d966cf_54ab98cde18245f08fe0678c374e2a01~mv2.png/v1/fill/w_119,h_117,al_c,q_85,usm_0.66_1.00_0.01,enc_auto/EC-%C3%81GUA-SANTA.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Guarani</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/guarani.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mirassol</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/mirassol.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Corinthians</t>
   </si>
   <si>
     <t xml:space="preserve">C</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/corinthians.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ferroviária</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/ferroviaria.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ituano</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/ituano.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">São Bento</t>
   </si>
   <si>
+    <t xml:space="preserve">https://ecsaobento.com.br/arquivos/logos/Sao-Bento-Sorocaba-01.svg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Palmeiras</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/palmeiras.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Portuguesa</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/portuguesa.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Santo André</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/santo_andre.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">São Bernardo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.escudosfc.com.br/images/sao_bernarndo_sp.png</t>
   </si>
 </sst>
 </file>
@@ -103,6 +154,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -120,7 +172,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,12 +183,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -174,16 +220,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -211,14 +253,14 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -231,199 +273,233 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="n">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>12816</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3"/>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>2698</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="n">
-        <v>2698</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="n">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>305</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="3"/>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="n">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>7789</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3"/>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3" t="n">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>12604</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3"/>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3" t="n">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>333</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3"/>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3" t="n">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>3865</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="3"/>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3" t="n">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>1207</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="3"/>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3" t="n">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>11064</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="3"/>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="3" t="n">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="n">
         <v>1039</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="3"/>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3" t="n">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="n">
         <v>1834</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="3"/>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="n">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2" t="n">
         <v>2028</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="3"/>
+      <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="3" t="n">
+      <c r="A14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2" t="n">
         <v>14584</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="3"/>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="3" t="n">
+      <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="n">
         <v>331</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="3"/>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="3" t="n">
+      <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="2" t="n">
         <v>370</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="3"/>
+      <c r="C16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="3" t="n">
+      <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="3"/>
+      <c r="C17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>